<commit_message>
feat: arreglo de fechas
</commit_message>
<xml_diff>
--- a/data/Metabase.xlsx
+++ b/data/Metabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\UCR-TEC\2025\Primer Semestre 2025\Estadística Actuarial I\TratamientoAgua\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93630F94-93BB-43DD-AC3A-0C02484B33AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FEC6F9-7F5B-4C09-A4F6-6286FF9649F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22944" yWindow="-1992" windowWidth="11232" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="2" r:id="rId1"/>
@@ -3031,7 +3031,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3092,6 +3092,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3105,7 +3111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3199,6 +3205,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3481,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="E197" sqref="E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3490,7 +3498,7 @@
     <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="131.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" customWidth="1"/>
     <col min="7" max="7" width="30.44140625" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
@@ -3760,7 +3768,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="34"/>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="41" t="s">
         <v>162</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -3780,7 +3788,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="34"/>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="41" t="s">
         <v>164</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -3800,7 +3808,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="34"/>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="41" t="s">
         <v>165</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -3902,7 +3910,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="34"/>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="41" t="s">
         <v>258</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -3942,7 +3950,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="34"/>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="41" t="s">
         <v>260</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -3962,7 +3970,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="34"/>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="41" t="s">
         <v>261</v>
       </c>
       <c r="E26" s="16" t="s">
@@ -3982,7 +3990,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="34"/>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="41" t="s">
         <v>262</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -4002,7 +4010,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="34"/>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="41" t="s">
         <v>264</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -4022,7 +4030,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="34"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="41" t="s">
         <v>265</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -4062,7 +4070,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="34"/>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="41" t="s">
         <v>267</v>
       </c>
       <c r="E31" s="16" t="s">
@@ -4102,7 +4110,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="34"/>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="41" t="s">
         <v>269</v>
       </c>
       <c r="E33" s="16" t="s">
@@ -4122,7 +4130,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="34"/>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="41" t="s">
         <v>270</v>
       </c>
       <c r="E34" s="16" t="s">
@@ -4224,7 +4232,7 @@
         <v>26</v>
       </c>
       <c r="C39" s="34"/>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="41" t="s">
         <v>275</v>
       </c>
       <c r="E39" s="16" t="s">
@@ -4404,7 +4412,7 @@
         <v>35</v>
       </c>
       <c r="C48" s="34"/>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="41" t="s">
         <v>285</v>
       </c>
       <c r="E48" s="16" t="s">
@@ -4424,7 +4432,7 @@
         <v>36</v>
       </c>
       <c r="C49" s="34"/>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="41" t="s">
         <v>286</v>
       </c>
       <c r="E49" s="16" t="s">
@@ -4444,7 +4452,7 @@
         <v>37</v>
       </c>
       <c r="C50" s="34"/>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="41" t="s">
         <v>287</v>
       </c>
       <c r="E50" s="16" t="s">
@@ -4464,7 +4472,7 @@
         <v>38</v>
       </c>
       <c r="C51" s="34"/>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="41" t="s">
         <v>288</v>
       </c>
       <c r="E51" s="16" t="s">
@@ -4484,7 +4492,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="34"/>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="41" t="s">
         <v>289</v>
       </c>
       <c r="E52" s="16" t="s">
@@ -4544,7 +4552,7 @@
         <v>42</v>
       </c>
       <c r="C55" s="34"/>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="41" t="s">
         <v>292</v>
       </c>
       <c r="E55" s="16" t="s">
@@ -4584,7 +4592,7 @@
         <v>44</v>
       </c>
       <c r="C57" s="34"/>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="41" t="s">
         <v>294</v>
       </c>
       <c r="E57" s="16" t="s">
@@ -4664,7 +4672,7 @@
         <v>48</v>
       </c>
       <c r="C61" s="34"/>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="41" t="s">
         <v>298</v>
       </c>
       <c r="E61" s="16" t="s">
@@ -4764,7 +4772,7 @@
         <v>52</v>
       </c>
       <c r="C66" s="34"/>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="41" t="s">
         <v>304</v>
       </c>
       <c r="E66" s="16" t="s">
@@ -4824,7 +4832,7 @@
         <v>55</v>
       </c>
       <c r="C69" s="34"/>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="41" t="s">
         <v>307</v>
       </c>
       <c r="E69" s="16" t="s">
@@ -4860,7 +4868,7 @@
       </c>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="14">
         <v>57</v>
@@ -4966,7 +4974,7 @@
         <v>62</v>
       </c>
       <c r="C76" s="34"/>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="41" t="s">
         <v>314</v>
       </c>
       <c r="E76" s="16" t="s">
@@ -5108,7 +5116,7 @@
       <c r="C83" s="33" t="s">
         <v>595</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="41" t="s">
         <v>321</v>
       </c>
       <c r="E83" s="16" t="s">
@@ -5148,7 +5156,7 @@
         <v>71</v>
       </c>
       <c r="C85" s="34"/>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="41" t="s">
         <v>323</v>
       </c>
       <c r="E85" s="16" t="s">
@@ -5188,7 +5196,7 @@
         <v>73</v>
       </c>
       <c r="C87" s="34"/>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="41" t="s">
         <v>325</v>
       </c>
       <c r="E87" s="16" t="s">
@@ -5228,7 +5236,7 @@
         <v>75</v>
       </c>
       <c r="C89" s="34"/>
-      <c r="D89" s="15" t="s">
+      <c r="D89" s="41" t="s">
         <v>327</v>
       </c>
       <c r="E89" s="16" t="s">
@@ -5268,7 +5276,7 @@
         <v>77</v>
       </c>
       <c r="C91" s="34"/>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="41" t="s">
         <v>329</v>
       </c>
       <c r="E91" s="16" t="s">
@@ -5308,7 +5316,7 @@
         <v>79</v>
       </c>
       <c r="C93" s="34"/>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="41" t="s">
         <v>331</v>
       </c>
       <c r="E93" s="16" t="s">
@@ -5350,7 +5358,7 @@
       <c r="C95" s="33" t="s">
         <v>608</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="41" t="s">
         <v>609</v>
       </c>
       <c r="E95" s="16" t="s">
@@ -5390,7 +5398,7 @@
         <v>83</v>
       </c>
       <c r="C97" s="34"/>
-      <c r="D97" s="15" t="s">
+      <c r="D97" s="41" t="s">
         <v>613</v>
       </c>
       <c r="E97" s="16" t="s">
@@ -5430,7 +5438,7 @@
         <v>85</v>
       </c>
       <c r="C99" s="34"/>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="41" t="s">
         <v>617</v>
       </c>
       <c r="E99" s="16" t="s">
@@ -5470,7 +5478,7 @@
         <v>87</v>
       </c>
       <c r="C101" s="34"/>
-      <c r="D101" s="15" t="s">
+      <c r="D101" s="41" t="s">
         <v>621</v>
       </c>
       <c r="E101" s="16" t="s">
@@ -5510,7 +5518,7 @@
         <v>89</v>
       </c>
       <c r="C103" s="34"/>
-      <c r="D103" s="15" t="s">
+      <c r="D103" s="41" t="s">
         <v>625</v>
       </c>
       <c r="E103" s="16" t="s">
@@ -5550,7 +5558,7 @@
         <v>91</v>
       </c>
       <c r="C105" s="34"/>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="41" t="s">
         <v>629</v>
       </c>
       <c r="E105" s="16" t="s">
@@ -5592,7 +5600,7 @@
       <c r="C107" s="33" t="s">
         <v>633</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D107" s="41" t="s">
         <v>634</v>
       </c>
       <c r="E107" s="16" t="s">
@@ -5612,7 +5620,7 @@
         <v>94</v>
       </c>
       <c r="C108" s="34"/>
-      <c r="D108" s="15" t="s">
+      <c r="D108" s="41" t="s">
         <v>636</v>
       </c>
       <c r="E108" s="16" t="s">
@@ -5791,7 +5799,7 @@
         <v>103</v>
       </c>
       <c r="C117" s="32"/>
-      <c r="D117" t="s">
+      <c r="D117" s="42" t="s">
         <v>383</v>
       </c>
       <c r="E117" t="s">
@@ -5812,7 +5820,7 @@
         <v>104</v>
       </c>
       <c r="C118" s="32"/>
-      <c r="D118" t="s">
+      <c r="D118" s="42" t="s">
         <v>384</v>
       </c>
       <c r="E118" t="s">
@@ -5854,7 +5862,7 @@
         <v>106</v>
       </c>
       <c r="C120" s="32"/>
-      <c r="D120" t="s">
+      <c r="D120" s="42" t="s">
         <v>392</v>
       </c>
       <c r="E120" t="s">
@@ -5875,7 +5883,7 @@
         <v>107</v>
       </c>
       <c r="C121" s="32"/>
-      <c r="D121" t="s">
+      <c r="D121" s="42" t="s">
         <v>393</v>
       </c>
       <c r="E121" t="s">
@@ -5896,7 +5904,7 @@
         <v>108</v>
       </c>
       <c r="C122" s="32"/>
-      <c r="D122" t="s">
+      <c r="D122" s="42" t="s">
         <v>394</v>
       </c>
       <c r="E122" t="s">
@@ -5917,7 +5925,7 @@
         <v>109</v>
       </c>
       <c r="C123" s="32"/>
-      <c r="D123" t="s">
+      <c r="D123" s="42" t="s">
         <v>395</v>
       </c>
       <c r="E123" t="s">
@@ -5938,7 +5946,7 @@
         <v>110</v>
       </c>
       <c r="C124" s="32"/>
-      <c r="D124" t="s">
+      <c r="D124" s="42" t="s">
         <v>396</v>
       </c>
       <c r="E124" t="s">
@@ -5980,7 +5988,7 @@
         <v>112</v>
       </c>
       <c r="C126" s="32"/>
-      <c r="D126" t="s">
+      <c r="D126" s="42" t="s">
         <v>398</v>
       </c>
       <c r="E126" t="s">
@@ -6001,7 +6009,7 @@
         <v>113</v>
       </c>
       <c r="C127" s="32"/>
-      <c r="D127" t="s">
+      <c r="D127" s="42" t="s">
         <v>402</v>
       </c>
       <c r="E127" t="s">
@@ -6043,7 +6051,7 @@
         <v>115</v>
       </c>
       <c r="C129" s="32"/>
-      <c r="D129" t="s">
+      <c r="D129" s="42" t="s">
         <v>457</v>
       </c>
       <c r="E129" t="s">
@@ -6064,7 +6072,7 @@
         <v>116</v>
       </c>
       <c r="C130" s="32"/>
-      <c r="D130" t="s">
+      <c r="D130" s="42" t="s">
         <v>458</v>
       </c>
       <c r="E130" t="s">
@@ -6106,7 +6114,7 @@
         <v>118</v>
       </c>
       <c r="C132" s="32"/>
-      <c r="D132" t="s">
+      <c r="D132" s="42" t="s">
         <v>465</v>
       </c>
       <c r="E132" t="s">
@@ -6127,7 +6135,7 @@
         <v>119</v>
       </c>
       <c r="C133" s="32"/>
-      <c r="D133" t="s">
+      <c r="D133" s="42" t="s">
         <v>466</v>
       </c>
       <c r="E133" t="s">
@@ -6148,7 +6156,7 @@
         <v>120</v>
       </c>
       <c r="C134" s="32"/>
-      <c r="D134" t="s">
+      <c r="D134" s="42" t="s">
         <v>467</v>
       </c>
       <c r="E134" t="s">
@@ -6169,7 +6177,7 @@
         <v>121</v>
       </c>
       <c r="C135" s="32"/>
-      <c r="D135" t="s">
+      <c r="D135" s="42" t="s">
         <v>468</v>
       </c>
       <c r="E135" t="s">
@@ -6190,7 +6198,7 @@
         <v>122</v>
       </c>
       <c r="C136" s="32"/>
-      <c r="D136" t="s">
+      <c r="D136" s="42" t="s">
         <v>469</v>
       </c>
       <c r="E136" t="s">
@@ -7120,8 +7128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:J97"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: manejo de NA
</commit_message>
<xml_diff>
--- a/data/Metabase.xlsx
+++ b/data/Metabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\UCR-TEC\2025\Primer Semestre 2025\Estadística Actuarial I\TratamientoAgua\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FEC6F9-7F5B-4C09-A4F6-6286FF9649F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D62773-BD1E-4563-9188-DDFAD4A30AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="-1992" windowWidth="11232" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-2100" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="2" r:id="rId1"/>
@@ -2922,7 +2922,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -3030,6 +3030,11 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3111,7 +3116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3184,6 +3189,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3205,8 +3212,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3489,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197"/>
+    <sheetView tabSelected="1" topLeftCell="E135" zoomScale="94" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,10 +3518,10 @@
         <v>486</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
@@ -3529,12 +3535,12 @@
       <c r="D2" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="37" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="39" t="s">
         <v>490</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3547,7 +3553,7 @@
       <c r="D3" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="4"/>
       <c r="G3" s="6" t="s">
         <v>494</v>
@@ -3565,7 +3571,7 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="4"/>
       <c r="G4" s="6" t="s">
         <v>498</v>
@@ -3585,7 +3591,7 @@
       <c r="D5" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="4"/>
       <c r="G5" s="6" t="s">
         <v>503</v>
@@ -3603,7 +3609,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="34"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="4"/>
       <c r="G6" s="6" t="s">
         <v>506</v>
@@ -3621,7 +3627,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="34"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="4"/>
       <c r="G7" s="6" t="s">
         <v>510</v>
@@ -3639,7 +3645,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="34"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="4"/>
       <c r="G8" s="6" t="s">
         <v>514</v>
@@ -3657,7 +3663,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="34"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="4"/>
       <c r="G9" s="6" t="s">
         <v>518</v>
@@ -3671,7 +3677,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="34"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="4"/>
       <c r="G10" s="6" t="s">
         <v>520</v>
@@ -3685,7 +3691,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="34"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -3727,7 +3733,7 @@
       <c r="B14" s="14">
         <v>1</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="35" t="s">
         <v>529</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -3749,17 +3755,17 @@
       <c r="B15" s="14">
         <v>2</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="15" t="s">
         <v>113</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="42" t="s">
         <v>533</v>
       </c>
-      <c r="G15" s="34"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
@@ -3767,8 +3773,8 @@
       <c r="B16" s="14">
         <v>3</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="32" t="s">
         <v>162</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -3787,8 +3793,8 @@
       <c r="B17" s="14">
         <v>4</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="36"/>
+      <c r="D17" s="32" t="s">
         <v>164</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -3807,8 +3813,8 @@
       <c r="B18" s="14">
         <v>5</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="41" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="32" t="s">
         <v>165</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -3827,7 +3833,7 @@
       <c r="B19" s="14">
         <v>6</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="15" t="s">
         <v>166</v>
       </c>
@@ -3842,12 +3848,12 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="14">
         <v>7</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="15" t="s">
         <v>193</v>
       </c>
@@ -3867,7 +3873,7 @@
       <c r="B21" s="14">
         <v>8</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="35" t="s">
         <v>540</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -3889,7 +3895,7 @@
       <c r="B22" s="14">
         <v>9</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="15" t="s">
         <v>223</v>
       </c>
@@ -3909,8 +3915,8 @@
       <c r="B23" s="14">
         <v>10</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="41" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="32" t="s">
         <v>258</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -3924,12 +3930,12 @@
       </c>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="14">
         <v>11</v>
       </c>
-      <c r="C24" s="34"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="15" t="s">
         <v>259</v>
       </c>
@@ -3949,8 +3955,8 @@
       <c r="B25" s="14">
         <v>12</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="41" t="s">
+      <c r="C25" s="36"/>
+      <c r="D25" s="32" t="s">
         <v>260</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -3969,8 +3975,8 @@
       <c r="B26" s="14">
         <v>13</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="41" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="32" t="s">
         <v>261</v>
       </c>
       <c r="E26" s="16" t="s">
@@ -3989,8 +3995,8 @@
       <c r="B27" s="14">
         <v>14</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="41" t="s">
+      <c r="C27" s="36"/>
+      <c r="D27" s="32" t="s">
         <v>262</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -4009,8 +4015,8 @@
       <c r="B28" s="14">
         <v>15</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="41" t="s">
+      <c r="C28" s="36"/>
+      <c r="D28" s="32" t="s">
         <v>264</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -4029,8 +4035,8 @@
       <c r="B29" s="14">
         <v>16</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="41" t="s">
+      <c r="C29" s="36"/>
+      <c r="D29" s="32" t="s">
         <v>265</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -4049,7 +4055,7 @@
       <c r="B30" s="14">
         <v>17</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="15" t="s">
         <v>266</v>
       </c>
@@ -4069,8 +4075,8 @@
       <c r="B31" s="14">
         <v>18</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="41" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="32" t="s">
         <v>267</v>
       </c>
       <c r="E31" s="16" t="s">
@@ -4089,7 +4095,7 @@
       <c r="B32" s="14">
         <v>19</v>
       </c>
-      <c r="C32" s="34"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="15" t="s">
         <v>268</v>
       </c>
@@ -4109,8 +4115,8 @@
       <c r="B33" s="14">
         <v>20</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="41" t="s">
+      <c r="C33" s="36"/>
+      <c r="D33" s="32" t="s">
         <v>269</v>
       </c>
       <c r="E33" s="16" t="s">
@@ -4129,8 +4135,8 @@
       <c r="B34" s="14">
         <v>21</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="41" t="s">
+      <c r="C34" s="36"/>
+      <c r="D34" s="32" t="s">
         <v>270</v>
       </c>
       <c r="E34" s="16" t="s">
@@ -4149,7 +4155,7 @@
       <c r="B35" s="14">
         <v>22</v>
       </c>
-      <c r="C35" s="34"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="15" t="s">
         <v>271</v>
       </c>
@@ -4169,7 +4175,7 @@
       <c r="B36" s="14">
         <v>23</v>
       </c>
-      <c r="C36" s="34"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="15" t="s">
         <v>272</v>
       </c>
@@ -4189,7 +4195,7 @@
       <c r="B37" s="14">
         <v>24</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="35" t="s">
         <v>553</v>
       </c>
       <c r="D37" s="15" t="s">
@@ -4211,7 +4217,7 @@
       <c r="B38" s="14">
         <v>25</v>
       </c>
-      <c r="C38" s="34"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="15" t="s">
         <v>274</v>
       </c>
@@ -4231,8 +4237,8 @@
       <c r="B39" s="14">
         <v>26</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="41" t="s">
+      <c r="C39" s="36"/>
+      <c r="D39" s="32" t="s">
         <v>275</v>
       </c>
       <c r="E39" s="16" t="s">
@@ -4251,7 +4257,7 @@
       <c r="B40" s="14">
         <v>27</v>
       </c>
-      <c r="C40" s="34"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="15" t="s">
         <v>276</v>
       </c>
@@ -4271,7 +4277,7 @@
       <c r="B41" s="14">
         <v>28</v>
       </c>
-      <c r="C41" s="34"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="15" t="s">
         <v>278</v>
       </c>
@@ -4291,7 +4297,7 @@
       <c r="B42" s="14">
         <v>29</v>
       </c>
-      <c r="C42" s="34"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="15" t="s">
         <v>279</v>
       </c>
@@ -4311,7 +4317,7 @@
       <c r="B43" s="14">
         <v>30</v>
       </c>
-      <c r="C43" s="34"/>
+      <c r="C43" s="36"/>
       <c r="D43" s="15" t="s">
         <v>280</v>
       </c>
@@ -4331,7 +4337,7 @@
       <c r="B44" s="14">
         <v>31</v>
       </c>
-      <c r="C44" s="34"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="15" t="s">
         <v>281</v>
       </c>
@@ -4351,7 +4357,7 @@
       <c r="B45" s="14">
         <v>32</v>
       </c>
-      <c r="C45" s="34"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="15" t="s">
         <v>282</v>
       </c>
@@ -4371,7 +4377,7 @@
       <c r="B46" s="14">
         <v>33</v>
       </c>
-      <c r="C46" s="34"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="15" t="s">
         <v>283</v>
       </c>
@@ -4391,7 +4397,7 @@
       <c r="B47" s="14">
         <v>34</v>
       </c>
-      <c r="C47" s="34"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="15" t="s">
         <v>284</v>
       </c>
@@ -4411,8 +4417,8 @@
       <c r="B48" s="14">
         <v>35</v>
       </c>
-      <c r="C48" s="34"/>
-      <c r="D48" s="41" t="s">
+      <c r="C48" s="36"/>
+      <c r="D48" s="32" t="s">
         <v>285</v>
       </c>
       <c r="E48" s="16" t="s">
@@ -4431,8 +4437,8 @@
       <c r="B49" s="14">
         <v>36</v>
       </c>
-      <c r="C49" s="34"/>
-      <c r="D49" s="41" t="s">
+      <c r="C49" s="36"/>
+      <c r="D49" s="32" t="s">
         <v>286</v>
       </c>
       <c r="E49" s="16" t="s">
@@ -4451,8 +4457,8 @@
       <c r="B50" s="14">
         <v>37</v>
       </c>
-      <c r="C50" s="34"/>
-      <c r="D50" s="41" t="s">
+      <c r="C50" s="36"/>
+      <c r="D50" s="32" t="s">
         <v>287</v>
       </c>
       <c r="E50" s="16" t="s">
@@ -4471,8 +4477,8 @@
       <c r="B51" s="14">
         <v>38</v>
       </c>
-      <c r="C51" s="34"/>
-      <c r="D51" s="41" t="s">
+      <c r="C51" s="36"/>
+      <c r="D51" s="32" t="s">
         <v>288</v>
       </c>
       <c r="E51" s="16" t="s">
@@ -4491,8 +4497,8 @@
       <c r="B52" s="14">
         <v>39</v>
       </c>
-      <c r="C52" s="34"/>
-      <c r="D52" s="41" t="s">
+      <c r="C52" s="36"/>
+      <c r="D52" s="32" t="s">
         <v>289</v>
       </c>
       <c r="E52" s="16" t="s">
@@ -4511,7 +4517,7 @@
       <c r="B53" s="14">
         <v>40</v>
       </c>
-      <c r="C53" s="34"/>
+      <c r="C53" s="36"/>
       <c r="D53" s="15" t="s">
         <v>290</v>
       </c>
@@ -4531,7 +4537,7 @@
       <c r="B54" s="14">
         <v>41</v>
       </c>
-      <c r="C54" s="34"/>
+      <c r="C54" s="36"/>
       <c r="D54" s="15" t="s">
         <v>291</v>
       </c>
@@ -4551,8 +4557,8 @@
       <c r="B55" s="14">
         <v>42</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="41" t="s">
+      <c r="C55" s="36"/>
+      <c r="D55" s="32" t="s">
         <v>292</v>
       </c>
       <c r="E55" s="16" t="s">
@@ -4571,7 +4577,7 @@
       <c r="B56" s="14">
         <v>43</v>
       </c>
-      <c r="C56" s="34"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="15" t="s">
         <v>293</v>
       </c>
@@ -4591,8 +4597,8 @@
       <c r="B57" s="14">
         <v>44</v>
       </c>
-      <c r="C57" s="34"/>
-      <c r="D57" s="41" t="s">
+      <c r="C57" s="36"/>
+      <c r="D57" s="32" t="s">
         <v>294</v>
       </c>
       <c r="E57" s="16" t="s">
@@ -4606,12 +4612,12 @@
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="14">
         <v>45</v>
       </c>
-      <c r="C58" s="34"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="15" t="s">
         <v>295</v>
       </c>
@@ -4631,7 +4637,7 @@
       <c r="B59" s="14">
         <v>46</v>
       </c>
-      <c r="C59" s="34"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="15" t="s">
         <v>296</v>
       </c>
@@ -4646,12 +4652,12 @@
       </c>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="14">
         <v>47</v>
       </c>
-      <c r="C60" s="34"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="15" t="s">
         <v>297</v>
       </c>
@@ -4666,13 +4672,13 @@
       </c>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="14">
         <v>48</v>
       </c>
-      <c r="C61" s="34"/>
-      <c r="D61" s="41" t="s">
+      <c r="C61" s="36"/>
+      <c r="D61" s="32" t="s">
         <v>298</v>
       </c>
       <c r="E61" s="16" t="s">
@@ -4691,7 +4697,7 @@
       <c r="B62" s="14">
         <v>50</v>
       </c>
-      <c r="C62" s="34"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="15" t="s">
         <v>300</v>
       </c>
@@ -4706,12 +4712,12 @@
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="14">
         <v>49</v>
       </c>
-      <c r="C63" s="34"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="15" t="s">
         <v>299</v>
       </c>
@@ -4726,12 +4732,12 @@
       </c>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="14">
         <v>50</v>
       </c>
-      <c r="C64" s="34"/>
+      <c r="C64" s="36"/>
       <c r="D64" s="15" t="s">
         <v>301</v>
       </c>
@@ -4751,7 +4757,7 @@
       <c r="B65" s="14">
         <v>51</v>
       </c>
-      <c r="C65" s="34"/>
+      <c r="C65" s="36"/>
       <c r="D65" s="15" t="s">
         <v>302</v>
       </c>
@@ -4771,8 +4777,8 @@
       <c r="B66" s="14">
         <v>52</v>
       </c>
-      <c r="C66" s="34"/>
-      <c r="D66" s="41" t="s">
+      <c r="C66" s="36"/>
+      <c r="D66" s="32" t="s">
         <v>304</v>
       </c>
       <c r="E66" s="16" t="s">
@@ -4791,7 +4797,7 @@
       <c r="B67" s="14">
         <v>53</v>
       </c>
-      <c r="C67" s="34"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="15" t="s">
         <v>305</v>
       </c>
@@ -4811,7 +4817,7 @@
       <c r="B68" s="14">
         <v>54</v>
       </c>
-      <c r="C68" s="34"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="15" t="s">
         <v>306</v>
       </c>
@@ -4831,8 +4837,8 @@
       <c r="B69" s="14">
         <v>55</v>
       </c>
-      <c r="C69" s="34"/>
-      <c r="D69" s="41" t="s">
+      <c r="C69" s="36"/>
+      <c r="D69" s="32" t="s">
         <v>307</v>
       </c>
       <c r="E69" s="16" t="s">
@@ -4851,7 +4857,7 @@
       <c r="B70" s="14">
         <v>56</v>
       </c>
-      <c r="C70" s="33" t="s">
+      <c r="C70" s="35" t="s">
         <v>584</v>
       </c>
       <c r="D70" s="15" t="s">
@@ -4868,12 +4874,12 @@
       </c>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="14">
         <v>57</v>
       </c>
-      <c r="C71" s="34"/>
+      <c r="C71" s="36"/>
       <c r="D71" s="15" t="s">
         <v>309</v>
       </c>
@@ -4893,7 +4899,7 @@
       <c r="B72" s="14">
         <v>58</v>
       </c>
-      <c r="C72" s="34"/>
+      <c r="C72" s="36"/>
       <c r="D72" s="15" t="s">
         <v>310</v>
       </c>
@@ -4913,7 +4919,7 @@
       <c r="B73" s="14">
         <v>59</v>
       </c>
-      <c r="C73" s="34"/>
+      <c r="C73" s="36"/>
       <c r="D73" s="15" t="s">
         <v>311</v>
       </c>
@@ -4933,7 +4939,7 @@
       <c r="B74" s="14">
         <v>60</v>
       </c>
-      <c r="C74" s="34"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="15" t="s">
         <v>312</v>
       </c>
@@ -4953,7 +4959,7 @@
       <c r="B75" s="14">
         <v>61</v>
       </c>
-      <c r="C75" s="34"/>
+      <c r="C75" s="36"/>
       <c r="D75" s="15" t="s">
         <v>313</v>
       </c>
@@ -4973,8 +4979,8 @@
       <c r="B76" s="14">
         <v>62</v>
       </c>
-      <c r="C76" s="34"/>
-      <c r="D76" s="41" t="s">
+      <c r="C76" s="36"/>
+      <c r="D76" s="32" t="s">
         <v>314</v>
       </c>
       <c r="E76" s="16" t="s">
@@ -4988,12 +4994,12 @@
       </c>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="14">
         <v>63</v>
       </c>
-      <c r="C77" s="34"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="15" t="s">
         <v>315</v>
       </c>
@@ -5013,7 +5019,7 @@
       <c r="B78" s="14">
         <v>64</v>
       </c>
-      <c r="C78" s="34"/>
+      <c r="C78" s="36"/>
       <c r="D78" s="15" t="s">
         <v>316</v>
       </c>
@@ -5033,7 +5039,7 @@
       <c r="B79" s="14">
         <v>65</v>
       </c>
-      <c r="C79" s="34"/>
+      <c r="C79" s="36"/>
       <c r="D79" s="15" t="s">
         <v>317</v>
       </c>
@@ -5053,7 +5059,7 @@
       <c r="B80" s="14">
         <v>66</v>
       </c>
-      <c r="C80" s="34"/>
+      <c r="C80" s="36"/>
       <c r="D80" s="15" t="s">
         <v>318</v>
       </c>
@@ -5073,7 +5079,7 @@
       <c r="B81" s="14">
         <v>67</v>
       </c>
-      <c r="C81" s="34"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="15" t="s">
         <v>319</v>
       </c>
@@ -5088,12 +5094,12 @@
       </c>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="14">
         <v>68</v>
       </c>
-      <c r="C82" s="34"/>
+      <c r="C82" s="36"/>
       <c r="D82" s="15" t="s">
         <v>320</v>
       </c>
@@ -5113,10 +5119,10 @@
       <c r="B83" s="14">
         <v>69</v>
       </c>
-      <c r="C83" s="33" t="s">
+      <c r="C83" s="35" t="s">
         <v>595</v>
       </c>
-      <c r="D83" s="41" t="s">
+      <c r="D83" s="32" t="s">
         <v>321</v>
       </c>
       <c r="E83" s="16" t="s">
@@ -5135,7 +5141,7 @@
       <c r="B84" s="14">
         <v>70</v>
       </c>
-      <c r="C84" s="34"/>
+      <c r="C84" s="36"/>
       <c r="D84" s="15" t="s">
         <v>322</v>
       </c>
@@ -5155,8 +5161,8 @@
       <c r="B85" s="14">
         <v>71</v>
       </c>
-      <c r="C85" s="34"/>
-      <c r="D85" s="41" t="s">
+      <c r="C85" s="36"/>
+      <c r="D85" s="32" t="s">
         <v>323</v>
       </c>
       <c r="E85" s="16" t="s">
@@ -5175,7 +5181,7 @@
       <c r="B86" s="14">
         <v>72</v>
       </c>
-      <c r="C86" s="34"/>
+      <c r="C86" s="36"/>
       <c r="D86" s="15" t="s">
         <v>324</v>
       </c>
@@ -5195,8 +5201,8 @@
       <c r="B87" s="14">
         <v>73</v>
       </c>
-      <c r="C87" s="34"/>
-      <c r="D87" s="41" t="s">
+      <c r="C87" s="36"/>
+      <c r="D87" s="32" t="s">
         <v>325</v>
       </c>
       <c r="E87" s="16" t="s">
@@ -5215,7 +5221,7 @@
       <c r="B88" s="14">
         <v>74</v>
       </c>
-      <c r="C88" s="34"/>
+      <c r="C88" s="36"/>
       <c r="D88" s="15" t="s">
         <v>326</v>
       </c>
@@ -5235,8 +5241,8 @@
       <c r="B89" s="14">
         <v>75</v>
       </c>
-      <c r="C89" s="34"/>
-      <c r="D89" s="41" t="s">
+      <c r="C89" s="36"/>
+      <c r="D89" s="32" t="s">
         <v>327</v>
       </c>
       <c r="E89" s="16" t="s">
@@ -5255,7 +5261,7 @@
       <c r="B90" s="14">
         <v>76</v>
       </c>
-      <c r="C90" s="34"/>
+      <c r="C90" s="36"/>
       <c r="D90" s="15" t="s">
         <v>328</v>
       </c>
@@ -5275,8 +5281,8 @@
       <c r="B91" s="14">
         <v>77</v>
       </c>
-      <c r="C91" s="34"/>
-      <c r="D91" s="41" t="s">
+      <c r="C91" s="36"/>
+      <c r="D91" s="32" t="s">
         <v>329</v>
       </c>
       <c r="E91" s="16" t="s">
@@ -5295,7 +5301,7 @@
       <c r="B92" s="14">
         <v>78</v>
       </c>
-      <c r="C92" s="34"/>
+      <c r="C92" s="36"/>
       <c r="D92" s="15" t="s">
         <v>330</v>
       </c>
@@ -5315,8 +5321,8 @@
       <c r="B93" s="14">
         <v>79</v>
       </c>
-      <c r="C93" s="34"/>
-      <c r="D93" s="41" t="s">
+      <c r="C93" s="36"/>
+      <c r="D93" s="32" t="s">
         <v>331</v>
       </c>
       <c r="E93" s="16" t="s">
@@ -5335,7 +5341,7 @@
       <c r="B94" s="14">
         <v>80</v>
       </c>
-      <c r="C94" s="34"/>
+      <c r="C94" s="36"/>
       <c r="D94" s="15" t="s">
         <v>332</v>
       </c>
@@ -5355,10 +5361,10 @@
       <c r="B95" s="14">
         <v>81</v>
       </c>
-      <c r="C95" s="33" t="s">
+      <c r="C95" s="35" t="s">
         <v>608</v>
       </c>
-      <c r="D95" s="41" t="s">
+      <c r="D95" s="32" t="s">
         <v>609</v>
       </c>
       <c r="E95" s="16" t="s">
@@ -5377,7 +5383,7 @@
       <c r="B96" s="14">
         <v>82</v>
       </c>
-      <c r="C96" s="34"/>
+      <c r="C96" s="36"/>
       <c r="D96" s="15" t="s">
         <v>611</v>
       </c>
@@ -5397,8 +5403,8 @@
       <c r="B97" s="14">
         <v>83</v>
       </c>
-      <c r="C97" s="34"/>
-      <c r="D97" s="41" t="s">
+      <c r="C97" s="36"/>
+      <c r="D97" s="32" t="s">
         <v>613</v>
       </c>
       <c r="E97" s="16" t="s">
@@ -5417,7 +5423,7 @@
       <c r="B98" s="14">
         <v>84</v>
       </c>
-      <c r="C98" s="34"/>
+      <c r="C98" s="36"/>
       <c r="D98" s="15" t="s">
         <v>615</v>
       </c>
@@ -5437,8 +5443,8 @@
       <c r="B99" s="14">
         <v>85</v>
       </c>
-      <c r="C99" s="34"/>
-      <c r="D99" s="41" t="s">
+      <c r="C99" s="36"/>
+      <c r="D99" s="32" t="s">
         <v>617</v>
       </c>
       <c r="E99" s="16" t="s">
@@ -5457,7 +5463,7 @@
       <c r="B100" s="14">
         <v>86</v>
       </c>
-      <c r="C100" s="34"/>
+      <c r="C100" s="36"/>
       <c r="D100" s="15" t="s">
         <v>619</v>
       </c>
@@ -5477,8 +5483,8 @@
       <c r="B101" s="14">
         <v>87</v>
       </c>
-      <c r="C101" s="34"/>
-      <c r="D101" s="41" t="s">
+      <c r="C101" s="36"/>
+      <c r="D101" s="32" t="s">
         <v>621</v>
       </c>
       <c r="E101" s="16" t="s">
@@ -5497,7 +5503,7 @@
       <c r="B102" s="14">
         <v>88</v>
       </c>
-      <c r="C102" s="34"/>
+      <c r="C102" s="36"/>
       <c r="D102" s="15" t="s">
         <v>623</v>
       </c>
@@ -5517,8 +5523,8 @@
       <c r="B103" s="14">
         <v>89</v>
       </c>
-      <c r="C103" s="34"/>
-      <c r="D103" s="41" t="s">
+      <c r="C103" s="36"/>
+      <c r="D103" s="32" t="s">
         <v>625</v>
       </c>
       <c r="E103" s="16" t="s">
@@ -5537,7 +5543,7 @@
       <c r="B104" s="14">
         <v>90</v>
       </c>
-      <c r="C104" s="34"/>
+      <c r="C104" s="36"/>
       <c r="D104" s="15" t="s">
         <v>627</v>
       </c>
@@ -5557,8 +5563,8 @@
       <c r="B105" s="14">
         <v>91</v>
       </c>
-      <c r="C105" s="34"/>
-      <c r="D105" s="41" t="s">
+      <c r="C105" s="36"/>
+      <c r="D105" s="32" t="s">
         <v>629</v>
       </c>
       <c r="E105" s="16" t="s">
@@ -5577,7 +5583,7 @@
       <c r="B106" s="14">
         <v>92</v>
       </c>
-      <c r="C106" s="34"/>
+      <c r="C106" s="36"/>
       <c r="D106" s="15" t="s">
         <v>631</v>
       </c>
@@ -5597,10 +5603,10 @@
       <c r="B107" s="14">
         <v>93</v>
       </c>
-      <c r="C107" s="33" t="s">
+      <c r="C107" s="35" t="s">
         <v>633</v>
       </c>
-      <c r="D107" s="41" t="s">
+      <c r="D107" s="32" t="s">
         <v>634</v>
       </c>
       <c r="E107" s="16" t="s">
@@ -5619,8 +5625,8 @@
       <c r="B108" s="14">
         <v>94</v>
       </c>
-      <c r="C108" s="34"/>
-      <c r="D108" s="41" t="s">
+      <c r="C108" s="36"/>
+      <c r="D108" s="32" t="s">
         <v>636</v>
       </c>
       <c r="E108" s="16" t="s">
@@ -5639,7 +5645,7 @@
       <c r="B109" s="14">
         <v>95</v>
       </c>
-      <c r="C109" s="34"/>
+      <c r="C109" s="36"/>
       <c r="D109" s="15" t="s">
         <v>346</v>
       </c>
@@ -5658,7 +5664,7 @@
       <c r="B110" s="14">
         <v>96</v>
       </c>
-      <c r="C110" s="32" t="s">
+      <c r="C110" s="34" t="s">
         <v>693</v>
       </c>
       <c r="D110" t="s">
@@ -5678,7 +5684,7 @@
       <c r="B111" s="14">
         <v>97</v>
       </c>
-      <c r="C111" s="32"/>
+      <c r="C111" s="34"/>
       <c r="D111" t="s">
         <v>162</v>
       </c>
@@ -5696,7 +5702,7 @@
       <c r="B112" s="14">
         <v>98</v>
       </c>
-      <c r="C112" s="32"/>
+      <c r="C112" s="34"/>
       <c r="D112" t="s">
         <v>0</v>
       </c>
@@ -5714,7 +5720,7 @@
       <c r="B113" s="14">
         <v>99</v>
       </c>
-      <c r="C113" s="32"/>
+      <c r="C113" s="34"/>
       <c r="D113" t="s">
         <v>349</v>
       </c>
@@ -5735,7 +5741,7 @@
       <c r="B114" s="14">
         <v>100</v>
       </c>
-      <c r="C114" s="32"/>
+      <c r="C114" s="34"/>
       <c r="D114" t="s">
         <v>351</v>
       </c>
@@ -5756,7 +5762,7 @@
       <c r="B115" s="14">
         <v>101</v>
       </c>
-      <c r="C115" s="32"/>
+      <c r="C115" s="34"/>
       <c r="D115" t="s">
         <v>358</v>
       </c>
@@ -5777,7 +5783,7 @@
       <c r="B116" s="14">
         <v>102</v>
       </c>
-      <c r="C116" s="32"/>
+      <c r="C116" s="34"/>
       <c r="D116" t="s">
         <v>376</v>
       </c>
@@ -5798,8 +5804,8 @@
       <c r="B117" s="14">
         <v>103</v>
       </c>
-      <c r="C117" s="32"/>
-      <c r="D117" s="42" t="s">
+      <c r="C117" s="34"/>
+      <c r="D117" s="33" t="s">
         <v>383</v>
       </c>
       <c r="E117" t="s">
@@ -5819,8 +5825,8 @@
       <c r="B118" s="14">
         <v>104</v>
       </c>
-      <c r="C118" s="32"/>
-      <c r="D118" s="42" t="s">
+      <c r="C118" s="34"/>
+      <c r="D118" s="33" t="s">
         <v>384</v>
       </c>
       <c r="E118" t="s">
@@ -5840,7 +5846,7 @@
       <c r="B119" s="14">
         <v>105</v>
       </c>
-      <c r="C119" s="32"/>
+      <c r="C119" s="34"/>
       <c r="D119" t="s">
         <v>386</v>
       </c>
@@ -5861,8 +5867,8 @@
       <c r="B120" s="14">
         <v>106</v>
       </c>
-      <c r="C120" s="32"/>
-      <c r="D120" s="42" t="s">
+      <c r="C120" s="34"/>
+      <c r="D120" s="33" t="s">
         <v>392</v>
       </c>
       <c r="E120" t="s">
@@ -5882,8 +5888,8 @@
       <c r="B121" s="14">
         <v>107</v>
       </c>
-      <c r="C121" s="32"/>
-      <c r="D121" s="42" t="s">
+      <c r="C121" s="34"/>
+      <c r="D121" s="33" t="s">
         <v>393</v>
       </c>
       <c r="E121" t="s">
@@ -5903,8 +5909,8 @@
       <c r="B122" s="14">
         <v>108</v>
       </c>
-      <c r="C122" s="32"/>
-      <c r="D122" s="42" t="s">
+      <c r="C122" s="34"/>
+      <c r="D122" s="33" t="s">
         <v>394</v>
       </c>
       <c r="E122" t="s">
@@ -5924,8 +5930,8 @@
       <c r="B123" s="14">
         <v>109</v>
       </c>
-      <c r="C123" s="32"/>
-      <c r="D123" s="42" t="s">
+      <c r="C123" s="34"/>
+      <c r="D123" s="33" t="s">
         <v>395</v>
       </c>
       <c r="E123" t="s">
@@ -5945,8 +5951,8 @@
       <c r="B124" s="14">
         <v>110</v>
       </c>
-      <c r="C124" s="32"/>
-      <c r="D124" s="42" t="s">
+      <c r="C124" s="34"/>
+      <c r="D124" s="33" t="s">
         <v>396</v>
       </c>
       <c r="E124" t="s">
@@ -5966,7 +5972,7 @@
       <c r="B125" s="14">
         <v>111</v>
       </c>
-      <c r="C125" s="32"/>
+      <c r="C125" s="34"/>
       <c r="D125" t="s">
         <v>670</v>
       </c>
@@ -5987,8 +5993,8 @@
       <c r="B126" s="14">
         <v>112</v>
       </c>
-      <c r="C126" s="32"/>
-      <c r="D126" s="42" t="s">
+      <c r="C126" s="34"/>
+      <c r="D126" s="33" t="s">
         <v>398</v>
       </c>
       <c r="E126" t="s">
@@ -6008,8 +6014,8 @@
       <c r="B127" s="14">
         <v>113</v>
       </c>
-      <c r="C127" s="32"/>
-      <c r="D127" s="42" t="s">
+      <c r="C127" s="34"/>
+      <c r="D127" s="33" t="s">
         <v>402</v>
       </c>
       <c r="E127" t="s">
@@ -6029,7 +6035,7 @@
       <c r="B128" s="14">
         <v>114</v>
       </c>
-      <c r="C128" s="32"/>
+      <c r="C128" s="34"/>
       <c r="D128" t="s">
         <v>451</v>
       </c>
@@ -6050,8 +6056,8 @@
       <c r="B129" s="14">
         <v>115</v>
       </c>
-      <c r="C129" s="32"/>
-      <c r="D129" s="42" t="s">
+      <c r="C129" s="34"/>
+      <c r="D129" s="33" t="s">
         <v>457</v>
       </c>
       <c r="E129" t="s">
@@ -6071,8 +6077,8 @@
       <c r="B130" s="14">
         <v>116</v>
       </c>
-      <c r="C130" s="32"/>
-      <c r="D130" s="42" t="s">
+      <c r="C130" s="34"/>
+      <c r="D130" s="33" t="s">
         <v>458</v>
       </c>
       <c r="E130" t="s">
@@ -6092,7 +6098,7 @@
       <c r="B131" s="14">
         <v>117</v>
       </c>
-      <c r="C131" s="32"/>
+      <c r="C131" s="34"/>
       <c r="D131" t="s">
         <v>459</v>
       </c>
@@ -6113,8 +6119,8 @@
       <c r="B132" s="14">
         <v>118</v>
       </c>
-      <c r="C132" s="32"/>
-      <c r="D132" s="42" t="s">
+      <c r="C132" s="34"/>
+      <c r="D132" s="33" t="s">
         <v>465</v>
       </c>
       <c r="E132" t="s">
@@ -6134,8 +6140,8 @@
       <c r="B133" s="14">
         <v>119</v>
       </c>
-      <c r="C133" s="32"/>
-      <c r="D133" s="42" t="s">
+      <c r="C133" s="34"/>
+      <c r="D133" s="33" t="s">
         <v>466</v>
       </c>
       <c r="E133" t="s">
@@ -6155,8 +6161,8 @@
       <c r="B134" s="14">
         <v>120</v>
       </c>
-      <c r="C134" s="32"/>
-      <c r="D134" s="42" t="s">
+      <c r="C134" s="34"/>
+      <c r="D134" s="33" t="s">
         <v>467</v>
       </c>
       <c r="E134" t="s">
@@ -6176,8 +6182,8 @@
       <c r="B135" s="14">
         <v>121</v>
       </c>
-      <c r="C135" s="32"/>
-      <c r="D135" s="42" t="s">
+      <c r="C135" s="34"/>
+      <c r="D135" s="33" t="s">
         <v>468</v>
       </c>
       <c r="E135" t="s">
@@ -6197,8 +6203,8 @@
       <c r="B136" s="14">
         <v>122</v>
       </c>
-      <c r="C136" s="32"/>
-      <c r="D136" s="42" t="s">
+      <c r="C136" s="34"/>
+      <c r="D136" s="33" t="s">
         <v>469</v>
       </c>
       <c r="E136" t="s">
@@ -6207,7 +6213,7 @@
       <c r="F136" t="s">
         <v>638</v>
       </c>
-      <c r="G136" t="s">
+      <c r="G136" s="43" t="s">
         <v>666</v>
       </c>
       <c r="H136" t="s">
@@ -6218,7 +6224,7 @@
       <c r="B137" s="14">
         <v>123</v>
       </c>
-      <c r="C137" s="32"/>
+      <c r="C137" s="34"/>
       <c r="D137" t="s">
         <v>691</v>
       </c>
@@ -7128,7 +7134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="A71" zoomScale="88" workbookViewId="0">
       <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>

</xml_diff>